<commit_message>
add scores to total rating excel
</commit_message>
<xml_diff>
--- a/evaluation/Total_rating.xlsx
+++ b/evaluation/Total_rating.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmlwl\Downloads\csci544-project\evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinszeto/Documents/USC/Fall2021/CSCI544/project/csci544-project/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F151A0-5D19-47FA-B8F5-FBA8CFE7890C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB42B99-4B4A-A14D-9BE9-A4B627493E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="1230" windowWidth="19926" windowHeight="3948" xr2:uid="{71DAF1CB-AE2B-4CC2-8937-EEE5B19B41DE}"/>
+    <workbookView xWindow="280" yWindow="460" windowWidth="12380" windowHeight="13460" xr2:uid="{71DAF1CB-AE2B-4CC2-8937-EEE5B19B41DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -71,14 +71,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -86,7 +86,7 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -129,7 +129,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -441,15 +441,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A80249-9428-4839-BFE0-F3F35EBDC52A}">
-  <dimension ref="A1:Q20"/>
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" topLeftCell="L2" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.7"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -501,8 +501,23 @@
       <c r="Q1" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R1" s="1">
+        <v>5</v>
+      </c>
+      <c r="S1" s="1">
+        <v>5</v>
+      </c>
+      <c r="T1" s="1">
+        <v>5</v>
+      </c>
+      <c r="U1" s="1">
+        <v>4</v>
+      </c>
+      <c r="V1" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -552,8 +567,23 @@
       <c r="Q2" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R2" s="1">
+        <v>3</v>
+      </c>
+      <c r="S2" s="1">
+        <v>3</v>
+      </c>
+      <c r="T2" s="1">
+        <v>3</v>
+      </c>
+      <c r="U2" s="1">
+        <v>3</v>
+      </c>
+      <c r="V2" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -603,8 +633,23 @@
       <c r="Q3" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R3" s="1">
+        <v>1</v>
+      </c>
+      <c r="S3" s="1">
+        <v>1</v>
+      </c>
+      <c r="T3" s="1">
+        <v>2</v>
+      </c>
+      <c r="U3" s="1">
+        <v>1</v>
+      </c>
+      <c r="V3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -654,8 +699,23 @@
       <c r="Q4" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" ht="30" x14ac:dyDescent="0.7">
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
+      <c r="S4" s="1">
+        <v>3</v>
+      </c>
+      <c r="T4" s="1">
+        <v>2</v>
+      </c>
+      <c r="U4" s="1">
+        <v>2</v>
+      </c>
+      <c r="V4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -707,8 +767,23 @@
       <c r="Q5" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R5" s="1">
+        <v>4</v>
+      </c>
+      <c r="S5" s="1">
+        <v>4</v>
+      </c>
+      <c r="T5" s="1">
+        <v>4</v>
+      </c>
+      <c r="U5" s="1">
+        <v>4</v>
+      </c>
+      <c r="V5" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -758,8 +833,23 @@
       <c r="Q6" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R6" s="1">
+        <v>3</v>
+      </c>
+      <c r="S6" s="1">
+        <v>2</v>
+      </c>
+      <c r="T6" s="1">
+        <v>3</v>
+      </c>
+      <c r="U6" s="1">
+        <v>2</v>
+      </c>
+      <c r="V6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="3"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -809,8 +899,23 @@
       <c r="Q7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R7" s="1">
+        <v>1</v>
+      </c>
+      <c r="S7" s="1">
+        <v>1</v>
+      </c>
+      <c r="T7" s="1">
+        <v>1</v>
+      </c>
+      <c r="U7" s="1">
+        <v>1</v>
+      </c>
+      <c r="V7" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -860,8 +965,23 @@
       <c r="Q8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" ht="45" x14ac:dyDescent="0.7">
+      <c r="R8" s="1">
+        <v>2</v>
+      </c>
+      <c r="S8" s="1">
+        <v>1</v>
+      </c>
+      <c r="T8" s="1">
+        <v>3</v>
+      </c>
+      <c r="U8" s="1">
+        <v>1</v>
+      </c>
+      <c r="V8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" ht="45" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -913,8 +1033,23 @@
       <c r="Q9" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R9" s="1">
+        <v>5</v>
+      </c>
+      <c r="S9" s="1">
+        <v>5</v>
+      </c>
+      <c r="T9" s="1">
+        <v>4</v>
+      </c>
+      <c r="U9" s="1">
+        <v>5</v>
+      </c>
+      <c r="V9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="2" t="s">
         <v>6</v>
@@ -964,8 +1099,23 @@
       <c r="Q10" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R10" s="1">
+        <v>3</v>
+      </c>
+      <c r="S10" s="1">
+        <v>3</v>
+      </c>
+      <c r="T10" s="1">
+        <v>4</v>
+      </c>
+      <c r="U10" s="1">
+        <v>3</v>
+      </c>
+      <c r="V10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="2" t="s">
         <v>7</v>
@@ -1015,8 +1165,23 @@
       <c r="Q11" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R11" s="1">
+        <v>1</v>
+      </c>
+      <c r="S11" s="1">
+        <v>1</v>
+      </c>
+      <c r="T11" s="1">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1">
+        <v>1</v>
+      </c>
+      <c r="V11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1066,8 +1231,23 @@
       <c r="Q12" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R12" s="1">
+        <v>3</v>
+      </c>
+      <c r="S12" s="1">
+        <v>3</v>
+      </c>
+      <c r="T12" s="1">
+        <v>3</v>
+      </c>
+      <c r="U12" s="1">
+        <v>2</v>
+      </c>
+      <c r="V12" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1119,8 +1299,23 @@
       <c r="Q13" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R13" s="1">
+        <v>4</v>
+      </c>
+      <c r="S13" s="1">
+        <v>5</v>
+      </c>
+      <c r="T13" s="1">
+        <v>5</v>
+      </c>
+      <c r="U13" s="1">
+        <v>4</v>
+      </c>
+      <c r="V13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
         <v>6</v>
@@ -1170,8 +1365,23 @@
       <c r="Q14" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R14" s="1">
+        <v>2</v>
+      </c>
+      <c r="S14" s="1">
+        <v>2</v>
+      </c>
+      <c r="T14" s="1">
+        <v>3</v>
+      </c>
+      <c r="U14" s="1">
+        <v>2</v>
+      </c>
+      <c r="V14" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="3"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
@@ -1221,8 +1431,23 @@
       <c r="Q15" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R15" s="1">
+        <v>1</v>
+      </c>
+      <c r="S15" s="1">
+        <v>1</v>
+      </c>
+      <c r="T15" s="1">
+        <v>2</v>
+      </c>
+      <c r="U15" s="1">
+        <v>1</v>
+      </c>
+      <c r="V15" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1272,8 +1497,23 @@
       <c r="Q16" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R16" s="1">
+        <v>2</v>
+      </c>
+      <c r="S16" s="1">
+        <v>3</v>
+      </c>
+      <c r="T16" s="1">
+        <v>3</v>
+      </c>
+      <c r="U16" s="1">
+        <v>2</v>
+      </c>
+      <c r="V16" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>4</v>
       </c>
@@ -1325,8 +1565,23 @@
       <c r="Q17" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R17" s="1">
+        <v>3</v>
+      </c>
+      <c r="S17" s="1">
+        <v>5</v>
+      </c>
+      <c r="T17" s="1">
+        <v>5</v>
+      </c>
+      <c r="U17" s="1">
+        <v>4</v>
+      </c>
+      <c r="V17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
@@ -1376,8 +1631,23 @@
       <c r="Q18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R18" s="1">
+        <v>2</v>
+      </c>
+      <c r="S18" s="1">
+        <v>2</v>
+      </c>
+      <c r="T18" s="1">
+        <v>3</v>
+      </c>
+      <c r="U18" s="1">
+        <v>2</v>
+      </c>
+      <c r="V18" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
@@ -1427,8 +1697,23 @@
       <c r="Q19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.7">
+      <c r="R19" s="1">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1">
+        <v>1</v>
+      </c>
+      <c r="T19" s="1">
+        <v>2</v>
+      </c>
+      <c r="U19" s="1">
+        <v>1</v>
+      </c>
+      <c r="V19" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="3"/>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -1477,6 +1762,21 @@
       </c>
       <c r="Q20" s="1">
         <v>1</v>
+      </c>
+      <c r="R20" s="1">
+        <v>2</v>
+      </c>
+      <c r="S20" s="1">
+        <v>3</v>
+      </c>
+      <c r="T20" s="1">
+        <v>3</v>
+      </c>
+      <c r="U20" s="1">
+        <v>2</v>
+      </c>
+      <c r="V20" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>